<commit_message>
added .gitignore, making updates for revision
</commit_message>
<xml_diff>
--- a/data/atlas_metadata_final.xlsx
+++ b/data/atlas_metadata_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbernabei/Documents/PhD_Research/atlas_project/iEEG_atlas_dev/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00188D0-0CEC-A24B-9266-B8178A51F775}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A8A615-D41B-D94E-A77F-83A9FF61D6B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12880" yWindow="1700" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
+    <workbookView xWindow="2880" yWindow="1260" windowWidth="25260" windowHeight="17720" xr2:uid="{55386E59-C2B1-FE47-8A03-2662CFD6A014}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="219">
   <si>
     <t>Patient</t>
   </si>
@@ -676,6 +676,12 @@
   </si>
   <si>
     <t>which_file</t>
+  </si>
+  <si>
+    <t>clip3_awake</t>
+  </si>
+  <si>
+    <t>clip4_awake</t>
   </si>
 </sst>
 </file>
@@ -717,9 +723,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEE15CE-15A7-E440-8B77-868E4F33ECBC}">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:U61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,11 +1063,10 @@
     <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1118,8 +1124,14 @@
       <c r="S1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T1" t="s">
+        <v>217</v>
+      </c>
+      <c r="U1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1177,8 +1189,14 @@
       <c r="S2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T2">
+        <v>423000</v>
+      </c>
+      <c r="U2">
+        <v>240179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1236,8 +1254,14 @@
       <c r="S3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T3">
+        <v>321431</v>
+      </c>
+      <c r="U3">
+        <v>440369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1295,8 +1319,14 @@
       <c r="S4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T4">
+        <v>496243</v>
+      </c>
+      <c r="U4">
+        <v>505225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1354,8 +1384,14 @@
       <c r="S5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T5">
+        <v>448787</v>
+      </c>
+      <c r="U5">
+        <v>323125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1413,8 +1449,14 @@
       <c r="S6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T6">
+        <v>452025</v>
+      </c>
+      <c r="U6">
+        <v>432781</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1472,8 +1514,14 @@
       <c r="S7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T7">
+        <v>307158</v>
+      </c>
+      <c r="U7">
+        <v>369859</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1531,8 +1579,14 @@
       <c r="S8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T8">
+        <v>337635</v>
+      </c>
+      <c r="U8">
+        <v>358854</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1590,8 +1644,14 @@
       <c r="S9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T9">
+        <v>394087</v>
+      </c>
+      <c r="U9">
+        <v>459399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1649,8 +1709,14 @@
       <c r="S10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T10">
+        <v>331745</v>
+      </c>
+      <c r="U10">
+        <v>503910</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -1708,8 +1774,14 @@
       <c r="S11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T11">
+        <v>312757</v>
+      </c>
+      <c r="U11">
+        <v>422265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1767,8 +1839,14 @@
       <c r="S12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T12">
+        <v>310000</v>
+      </c>
+      <c r="U12">
+        <v>421505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1826,8 +1904,14 @@
       <c r="S13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T13">
+        <v>335115</v>
+      </c>
+      <c r="U13">
+        <v>498400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1885,8 +1969,14 @@
       <c r="S14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T14">
+        <v>272510</v>
+      </c>
+      <c r="U14">
+        <v>281330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -1944,8 +2034,14 @@
       <c r="S15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T15">
+        <v>400027</v>
+      </c>
+      <c r="U15">
+        <v>521203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2003,8 +2099,14 @@
       <c r="S16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T16">
+        <v>626005</v>
+      </c>
+      <c r="U16">
+        <v>717104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -2062,8 +2164,14 @@
       <c r="S17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T17">
+        <v>481075</v>
+      </c>
+      <c r="U17">
+        <v>626864</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2121,8 +2229,14 @@
       <c r="S18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T18">
+        <v>403456</v>
+      </c>
+      <c r="U18">
+        <v>494683</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2180,8 +2294,14 @@
       <c r="S19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T19">
+        <v>372001</v>
+      </c>
+      <c r="U19">
+        <v>458761</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2239,8 +2359,14 @@
       <c r="S20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T20">
+        <v>339000</v>
+      </c>
+      <c r="U20">
+        <v>506000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>210</v>
       </c>
@@ -2298,8 +2424,14 @@
       <c r="S21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T21">
+        <v>283794</v>
+      </c>
+      <c r="U21">
+        <v>307000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>213</v>
       </c>
@@ -2357,8 +2489,14 @@
       <c r="S22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T22">
+        <v>328949</v>
+      </c>
+      <c r="U22">
+        <v>413970</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2416,8 +2554,14 @@
       <c r="S23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T23">
+        <v>419000</v>
+      </c>
+      <c r="U23">
+        <v>442000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>207</v>
       </c>
@@ -2475,8 +2619,14 @@
       <c r="S24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T24">
+        <v>234000</v>
+      </c>
+      <c r="U24">
+        <v>272257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2534,8 +2684,14 @@
       <c r="S25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T25">
+        <v>251969</v>
+      </c>
+      <c r="U25">
+        <v>320099</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2593,8 +2749,14 @@
       <c r="S26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T26">
+        <v>616000</v>
+      </c>
+      <c r="U26">
+        <v>750040</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -2652,8 +2814,14 @@
       <c r="S27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T27">
+        <v>185000</v>
+      </c>
+      <c r="U27">
+        <v>283000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -2711,8 +2879,14 @@
       <c r="S28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T28" s="2">
+        <v>265849</v>
+      </c>
+      <c r="U28" s="2">
+        <v>345020</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2770,8 +2944,14 @@
       <c r="S29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T29">
+        <v>364504</v>
+      </c>
+      <c r="U29" s="2">
+        <v>419000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -2829,8 +3009,14 @@
       <c r="S30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T30">
+        <v>348999</v>
+      </c>
+      <c r="U30">
+        <v>415000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -2888,8 +3074,14 @@
       <c r="S31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T31">
+        <v>367000</v>
+      </c>
+      <c r="U31">
+        <v>407000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -2947,8 +3139,14 @@
       <c r="S32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T32">
+        <v>352000</v>
+      </c>
+      <c r="U32">
+        <v>428018</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -3006,8 +3204,14 @@
       <c r="S33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T33">
+        <v>574000</v>
+      </c>
+      <c r="U33">
+        <v>507342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -3065,8 +3269,14 @@
       <c r="S34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T34">
+        <v>344160</v>
+      </c>
+      <c r="U34">
+        <v>524829</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -3124,8 +3334,14 @@
       <c r="S35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T35">
+        <v>311000</v>
+      </c>
+      <c r="U35">
+        <v>385000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -3183,8 +3399,14 @@
       <c r="S36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T36">
+        <v>337043</v>
+      </c>
+      <c r="U36">
+        <v>413000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -3242,8 +3464,14 @@
       <c r="S37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T37">
+        <v>378000</v>
+      </c>
+      <c r="U37">
+        <v>458000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -3301,8 +3529,14 @@
       <c r="S38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T38">
+        <v>330000</v>
+      </c>
+      <c r="U38">
+        <v>351360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -3360,8 +3594,14 @@
       <c r="S39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T39">
+        <v>456000</v>
+      </c>
+      <c r="U39">
+        <v>1082204</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -3419,8 +3659,14 @@
       <c r="S40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T40">
+        <v>200000</v>
+      </c>
+      <c r="U40">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -3478,8 +3724,14 @@
       <c r="S41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T41">
+        <v>337000</v>
+      </c>
+      <c r="U41">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -3537,8 +3789,14 @@
       <c r="S42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T42">
+        <v>287976</v>
+      </c>
+      <c r="U42">
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -3596,8 +3854,14 @@
       <c r="S43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T43">
+        <v>336000</v>
+      </c>
+      <c r="U43">
+        <v>424000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -3655,8 +3919,14 @@
       <c r="S44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T44">
+        <v>356000</v>
+      </c>
+      <c r="U44">
+        <v>510000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -3714,8 +3984,14 @@
       <c r="S45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T45">
+        <v>338000</v>
+      </c>
+      <c r="U45">
+        <v>430000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -3773,8 +4049,14 @@
       <c r="S46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T46">
+        <v>360000</v>
+      </c>
+      <c r="U46">
+        <v>410000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -3832,8 +4114,14 @@
       <c r="S47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T47">
+        <v>297500</v>
+      </c>
+      <c r="U47">
+        <v>367000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -3891,8 +4179,14 @@
       <c r="S48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T48">
+        <v>510085</v>
+      </c>
+      <c r="U48">
+        <v>563000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -3906,7 +4200,7 @@
         <v>1.4</v>
       </c>
       <c r="E49">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="F49" t="s">
         <v>120</v>
@@ -3950,8 +4244,14 @@
       <c r="S49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T49">
+        <v>815001</v>
+      </c>
+      <c r="U49">
+        <v>986400</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -4009,8 +4309,14 @@
       <c r="S50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T50">
+        <v>395000</v>
+      </c>
+      <c r="U50">
+        <v>462000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -4068,8 +4374,14 @@
       <c r="S51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T51">
+        <v>335000</v>
+      </c>
+      <c r="U51">
+        <v>415000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -4127,8 +4439,14 @@
       <c r="S52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T52">
+        <v>340000</v>
+      </c>
+      <c r="U52">
+        <v>480000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -4186,8 +4504,14 @@
       <c r="S53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T53">
+        <v>261000</v>
+      </c>
+      <c r="U53">
+        <v>324000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -4245,8 +4569,14 @@
       <c r="S54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T54">
+        <v>367000</v>
+      </c>
+      <c r="U54">
+        <v>520000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -4304,8 +4634,14 @@
       <c r="S55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T55">
+        <v>349000</v>
+      </c>
+      <c r="U55">
+        <v>432000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -4363,8 +4699,14 @@
       <c r="S56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T56">
+        <v>270000</v>
+      </c>
+      <c r="U56">
+        <v>455000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -4422,8 +4764,14 @@
       <c r="S57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T57">
+        <v>106000</v>
+      </c>
+      <c r="U57">
+        <v>46671</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -4481,8 +4829,14 @@
       <c r="S58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T58">
+        <v>266000</v>
+      </c>
+      <c r="U58">
+        <v>303000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -4540,8 +4894,14 @@
       <c r="S59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T59">
+        <v>349000</v>
+      </c>
+      <c r="U59">
+        <v>424800</v>
+      </c>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>53</v>
       </c>
@@ -4599,8 +4959,14 @@
       <c r="S60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T60">
+        <v>401000</v>
+      </c>
+      <c r="U60">
+        <v>329000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>54</v>
       </c>
@@ -4657,6 +5023,12 @@
       </c>
       <c r="S61">
         <v>1</v>
+      </c>
+      <c r="T61">
+        <v>356000</v>
+      </c>
+      <c r="U61">
+        <v>443928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>